<commit_message>
Elaboración de plantilla para sobre 1 y dossier publicitario
</commit_message>
<xml_diff>
--- a/Práctica 3/Product Backlog.xlsx
+++ b/Práctica 3/Product Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Asignaturas\3er Curso\1er Cuatrimestre\PSG\Prácticas\Práctica 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F7CD42A-0F87-4C74-B779-43DE795B49A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6011049A-EB3E-4788-B04C-95D1A9EBFA1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{712692D0-2489-4A8B-AD1C-6C5A8149080F}"/>
   </bookViews>
@@ -472,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24636678-4BF6-436B-8650-A3E0BAA406A5}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -488,7 +488,7 @@
     <col min="6" max="6" width="8.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -519,7 +519,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="1">
-        <v>18</v>
+        <v>35</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -533,7 +536,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="1">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -547,7 +553,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="1">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -561,7 +570,10 @@
         <v>4</v>
       </c>
       <c r="D5" s="1">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -575,7 +587,10 @@
         <v>5</v>
       </c>
       <c r="D6" s="1">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -588,6 +603,12 @@
       <c r="C7" s="1">
         <v>6</v>
       </c>
+      <c r="D7" s="1">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -599,6 +620,12 @@
       <c r="C8" s="1">
         <v>7</v>
       </c>
+      <c r="D8" s="1">
+        <v>10</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -610,6 +637,12 @@
       <c r="C9" s="1">
         <v>8</v>
       </c>
+      <c r="D9" s="1">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -621,6 +654,12 @@
       <c r="C10" s="1">
         <v>9</v>
       </c>
+      <c r="D10" s="1">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -632,6 +671,12 @@
       <c r="C11" s="1">
         <v>10</v>
       </c>
+      <c r="D11" s="1">
+        <v>15</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -643,6 +688,12 @@
       <c r="C12" s="1">
         <v>11</v>
       </c>
+      <c r="D12" s="1">
+        <v>15</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -654,6 +705,12 @@
       <c r="C13" s="1">
         <v>12</v>
       </c>
+      <c r="D13" s="1">
+        <v>15</v>
+      </c>
+      <c r="F13" s="1">
+        <v>3</v>
+      </c>
       <c r="G13" t="s">
         <v>27</v>
       </c>
@@ -668,6 +725,12 @@
       <c r="C14" s="1">
         <v>13</v>
       </c>
+      <c r="D14" s="1">
+        <v>5</v>
+      </c>
+      <c r="F14" s="1">
+        <v>3</v>
+      </c>
       <c r="G14" t="s">
         <v>27</v>
       </c>
@@ -682,6 +745,12 @@
       <c r="C15" s="1">
         <v>14</v>
       </c>
+      <c r="D15" s="1">
+        <v>5</v>
+      </c>
+      <c r="F15" s="1">
+        <v>3</v>
+      </c>
       <c r="G15" t="s">
         <v>27</v>
       </c>
@@ -696,8 +765,14 @@
       <c r="C16" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="1">
+        <v>5</v>
+      </c>
+      <c r="F16" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>7</v>
       </c>
@@ -707,8 +782,14 @@
       <c r="C17" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="1">
+        <v>5</v>
+      </c>
+      <c r="F17" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>8</v>
       </c>
@@ -721,8 +802,11 @@
       <c r="D18" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F18" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>9</v>
       </c>
@@ -735,8 +819,11 @@
       <c r="D19" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F19" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>11</v>
       </c>
@@ -749,8 +836,11 @@
       <c r="D20" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F20" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>10</v>
       </c>
@@ -761,10 +851,13 @@
         <v>20</v>
       </c>
       <c r="D21" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="F21" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -775,7 +868,16 @@
         <v>21</v>
       </c>
       <c r="D22" s="1">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="F22" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D23" s="1">
+        <f>SUM(D2:D22)</f>
+        <v>248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Primer sprint de práctica 3
</commit_message>
<xml_diff>
--- a/Práctica 3/Product Backlog.xlsx
+++ b/Práctica 3/Product Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Asignaturas\3er Curso\1er Cuatrimestre\PSG\Prácticas\Práctica 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferna\Desktop\Universidad\PSG I\proyectoPSG\Práctica 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6011049A-EB3E-4788-B04C-95D1A9EBFA1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA992236-2D42-423D-BEAC-FDB1C2070256}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{712692D0-2489-4A8B-AD1C-6C5A8149080F}"/>
+    <workbookView xWindow="75" yWindow="3075" windowWidth="15375" windowHeight="7995" xr2:uid="{712692D0-2489-4A8B-AD1C-6C5A8149080F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -153,10 +156,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -475,20 +481,20 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.21875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,7 +514,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -524,8 +530,11 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -541,8 +550,11 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -558,8 +570,11 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -576,7 +591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -593,7 +608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>14</v>
       </c>
@@ -610,7 +625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>16</v>
       </c>
@@ -627,7 +642,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>17</v>
       </c>
@@ -644,7 +659,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>15</v>
       </c>
@@ -661,7 +676,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>12</v>
       </c>
@@ -678,7 +693,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>13</v>
       </c>
@@ -695,7 +710,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>19</v>
       </c>
@@ -715,7 +730,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>20</v>
       </c>
@@ -735,7 +750,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>21</v>
       </c>
@@ -755,7 +770,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>6</v>
       </c>
@@ -772,7 +787,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>7</v>
       </c>
@@ -789,7 +804,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>8</v>
       </c>
@@ -806,7 +821,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>9</v>
       </c>
@@ -823,7 +838,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>11</v>
       </c>
@@ -840,7 +855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>10</v>
       </c>
@@ -857,7 +872,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -874,7 +889,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D23" s="1">
         <f>SUM(D2:D22)</f>
         <v>248</v>

</xml_diff>

<commit_message>
Actualización del product backlog
</commit_message>
<xml_diff>
--- a/Práctica 3/Product Backlog.xlsx
+++ b/Práctica 3/Product Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferna\Desktop\Universidad\PSG I\proyectoPSG\Práctica 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA992236-2D42-423D-BEAC-FDB1C2070256}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA193385-3C47-42E1-9379-350D6F670B9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="3075" windowWidth="15375" windowHeight="7995" xr2:uid="{712692D0-2489-4A8B-AD1C-6C5A8149080F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{712692D0-2489-4A8B-AD1C-6C5A8149080F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -481,7 +481,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,6 +590,9 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
+      <c r="G5" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -607,6 +610,9 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
+      <c r="G6" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -786,8 +792,11 @@
       <c r="F16" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>7</v>
       </c>
@@ -803,8 +812,11 @@
       <c r="F17" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>8</v>
       </c>
@@ -820,8 +832,11 @@
       <c r="F18" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G18" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>9</v>
       </c>
@@ -837,8 +852,11 @@
       <c r="F19" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>11</v>
       </c>
@@ -854,8 +872,11 @@
       <c r="F20" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>10</v>
       </c>
@@ -871,8 +892,11 @@
       <c r="F21" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -889,7 +913,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D23" s="1">
         <f>SUM(D2:D22)</f>
         <v>248</v>

</xml_diff>